<commit_message>
Turned off smart identification for the final status object
</commit_message>
<xml_diff>
--- a/uft-one-traditional-or-ppm-standards-review-create-project/Default.xlsx
+++ b/uft-one-traditional-or-ppm-standards-review-create-project/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -520,15 +520,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>